<commit_message>
Commit by Scrum Master
</commit_message>
<xml_diff>
--- a/AutomationExecrcise/src/test/resources/TestData.xlsx
+++ b/AutomationExecrcise/src/test/resources/TestData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\Programs\Java Programs\Eclipse\AutomationExecrcise\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\AutomationExecrcise\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B376DFF-2E3F-4E41-9585-500003032735}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D4ECB80-9F15-4696-B5E9-2D37FE0BA2A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Create Account" sheetId="1" r:id="rId1"/>
@@ -30,13 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="125">
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="123">
   <si>
     <t>Aditya</t>
   </si>
@@ -179,21 +173,6 @@
     <t>Mrs.</t>
   </si>
   <si>
-    <t>Name on card</t>
-  </si>
-  <si>
-    <t>Card Number</t>
-  </si>
-  <si>
-    <t>CVC</t>
-  </si>
-  <si>
-    <t>Expiration Month</t>
-  </si>
-  <si>
-    <t>Expiration Year</t>
-  </si>
-  <si>
     <t xml:space="preserve">Aditya </t>
   </si>
   <si>
@@ -218,9 +197,6 @@
     <t>Dress</t>
   </si>
   <si>
-    <t>Tops</t>
-  </si>
-  <si>
     <t>Saree</t>
   </si>
   <si>
@@ -233,9 +209,6 @@
     <t>Tops &amp; Shirts</t>
   </si>
   <si>
-    <t>Add Review</t>
-  </si>
-  <si>
     <t>"Great product! Fast delivery and excellent quality. Highly recommend!"</t>
   </si>
   <si>
@@ -405,6 +378,27 @@
   </si>
   <si>
     <t>D:\Study\Programs\Java Programs\Eclipse\AutomationExecrcise\Screenshot\4.png</t>
+  </si>
+  <si>
+    <t>Top</t>
+  </si>
+  <si>
+    <t>Add Review(2)</t>
+  </si>
+  <si>
+    <t>Name on card(0)</t>
+  </si>
+  <si>
+    <t>Card Number(1)</t>
+  </si>
+  <si>
+    <t>CVC(2)</t>
+  </si>
+  <si>
+    <t>Expiration Month(3)</t>
+  </si>
+  <si>
+    <t>Expiration Year(4)</t>
   </si>
 </sst>
 </file>
@@ -838,102 +832,102 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="J1" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="K1" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="L1" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="M1" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="N1" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="O1" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="P1" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="Q1" s="6" t="s">
         <v>89</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="M1" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="N1" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="O1" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="P1" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="Q1" s="6" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E2" s="1">
         <v>8</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G2" s="1">
         <v>2000</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O2" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="P2" s="1">
         <v>500084</v>
@@ -944,49 +938,49 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="E3" s="1">
         <v>10</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G3" s="1">
         <v>2001</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="M3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="O3" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="P3" s="1">
         <v>300041</v>
@@ -997,49 +991,49 @@
     </row>
     <row r="4" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="E4" s="2">
         <v>15</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G4" s="2">
         <v>1998</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="I4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K4" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="L4" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="K4" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="M4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="O4" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="N4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="O4" s="2" t="s">
-        <v>12</v>
       </c>
       <c r="P4" s="2">
         <v>500081</v>
@@ -1050,49 +1044,49 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>34</v>
       </c>
       <c r="E5" s="1">
         <v>22</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G5" s="1">
         <v>1995</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="I5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K5" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="L5" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="K5" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="M5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O5" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="O5" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="P5" s="1">
         <v>500034</v>
@@ -1103,49 +1097,49 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="E6" s="1">
         <v>5</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G6" s="1">
         <v>1999</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K6" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="L6" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="K6" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>47</v>
-      </c>
       <c r="M6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O6" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="O6" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="P6" s="1">
         <v>500032</v>
@@ -1189,155 +1183,155 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="J1" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="B1" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="C1" s="6" t="s">
+      <c r="K1" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="M1" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="N1" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="O1" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="P1" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="Q1" s="6" t="s">
         <v>89</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="M1" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="N1" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="O1" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="P1" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="Q1" s="6" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>101</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>110</v>
       </c>
       <c r="E2" s="1">
         <v>8</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G2" s="1">
         <v>2000</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O2" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="P2" s="1">
         <v>500084</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="E3" s="1">
         <v>10</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G3" s="1">
         <v>2001</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="M3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="O3" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="P3" s="1">
         <v>300041</v>
@@ -1348,49 +1342,49 @@
     </row>
     <row r="4" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="E4" s="2">
         <v>15</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G4" s="2">
         <v>1998</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="I4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K4" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="L4" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="K4" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="M4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="O4" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="N4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="O4" s="2" t="s">
-        <v>12</v>
       </c>
       <c r="P4" s="2">
         <v>500081</v>
@@ -1401,49 +1395,49 @@
     </row>
     <row r="5" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="E5" s="1">
         <v>22</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G5" s="1">
         <v>1995</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="I5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K5" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="L5" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="K5" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="M5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O5" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="O5" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="P5" s="1">
         <v>500034</v>
@@ -1454,49 +1448,49 @@
     </row>
     <row r="6" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="E6" s="1">
         <v>5</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G6" s="1">
         <v>1999</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K6" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="L6" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="K6" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>47</v>
-      </c>
       <c r="M6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O6" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="O6" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="P6" s="1">
         <v>500032</v>
@@ -1516,7 +1510,7 @@
   <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1526,42 +1520,42 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>62</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1574,7 +1568,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1585,68 +1579,68 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>0</v>
+        <v>74</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>1</v>
+        <v>75</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>67</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1663,41 +1657,42 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{526A9393-80B9-4F62-A5C9-5D7A0A4D8D96}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.109375" customWidth="1"/>
     <col min="2" max="2" width="22.77734375" customWidth="1"/>
-    <col min="4" max="4" width="15.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" customWidth="1"/>
+    <col min="5" max="5" width="22.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>49</v>
+        <v>118</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>50</v>
+        <v>119</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>51</v>
+        <v>120</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>52</v>
+        <v>121</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>53</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="C2" s="4">
         <v>123</v>
@@ -1711,10 +1706,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="C3" s="4">
         <v>456</v>
@@ -1728,10 +1723,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="C4" s="4">
         <v>789</v>
@@ -1745,10 +1740,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="C5" s="4">
         <v>234</v>
@@ -1762,10 +1757,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="C6" s="4">
         <v>567</v>
@@ -1786,7 +1781,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE8EB86F-9D4D-4FAE-A006-E375026A509D}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
@@ -1800,104 +1795,104 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>